<commit_message>
实现条文GB51251_2017_4_5_2 GB51251_2017_4_5_2 GB51251_2017_4_4_10 GB50067_2014_8_2_1 GB50067_2014_8_2_2 GB50157_2013_28_4_2 GB50490_2009_8_4_19  GB50736_2012_6_3_6 GB50157_2013_28_4_22
</commit_message>
<xml_diff>
--- a/UnitTestHVACChecker/测试数据/测试数据.xlsx
+++ b/UnitTestHVACChecker/测试数据/测试数据.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="18255" windowHeight="7080" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="18260" windowHeight="7080" firstSheet="11" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="不同顺序系统类型" sheetId="1" r:id="rId1"/>
@@ -947,16 +947,16 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -990,7 +990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1034,27 +1034,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="A1:Q18"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>99</v>
       </c>
       <c r="L10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>99</v>
       </c>
       <c r="L11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>99</v>
       </c>
       <c r="L12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1690,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2018,26 +2018,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>30</v>
       </c>
       <c r="L9" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
@@ -2525,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>30</v>
       </c>
       <c r="L15" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15" s="4">
         <v>2</v>
@@ -2849,7 +2849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>30</v>
       </c>
       <c r="L21" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M21" s="6">
         <v>2</v>
@@ -3184,26 +3184,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="J19" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>30</v>
       </c>
       <c r="L9" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
@@ -3707,7 +3707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3931,7 +3931,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>30</v>
       </c>
       <c r="L15" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15" s="4">
         <v>2</v>
@@ -4043,7 +4043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -4099,7 +4099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="6" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>30</v>
       </c>
       <c r="L21" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M21" s="6">
         <v>2</v>
@@ -4379,7 +4379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -4435,7 +4435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -4547,7 +4547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>30</v>
       </c>
       <c r="L27" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M27" s="4">
         <v>2</v>
@@ -4726,26 +4726,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="J13" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5137,7 +5137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="2" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" s="2" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>30</v>
       </c>
       <c r="L9" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="2">
         <v>1</v>
@@ -5249,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -5305,7 +5305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>30</v>
       </c>
       <c r="L15" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M15" s="4">
         <v>2</v>
@@ -5585,7 +5585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -5809,7 +5809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:18" s="6" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" s="6" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>30</v>
       </c>
       <c r="L21" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M21" s="6">
         <v>2</v>
@@ -5921,7 +5921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -6145,7 +6145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:18" s="4" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -6216,18 +6216,18 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.375" customWidth="1"/>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="24.625" customWidth="1"/>
-    <col min="7" max="7" width="13.75" customWidth="1"/>
+    <col min="6" max="6" width="24.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>135</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6273,7 +6273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6329,23 +6329,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="19.125" customWidth="1"/>
-    <col min="8" max="8" width="10.125" customWidth="1"/>
-    <col min="9" max="9" width="70.375" customWidth="1"/>
-    <col min="10" max="10" width="13.375" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" customWidth="1"/>
+    <col min="9" max="9" width="70.36328125" customWidth="1"/>
+    <col min="10" max="10" width="13.36328125" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="56" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="56" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" ht="56" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -6726,27 +6726,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="17.75" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="10.375" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7148,28 +7148,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView topLeftCell="I7" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
-    <col min="18" max="18" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
+    <col min="18" max="18" width="16.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -7225,7 +7225,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7281,7 +7281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7393,7 +7393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" ht="28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7505,7 +7505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7617,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7785,7 +7785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7841,7 +7841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7953,7 +7953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>500</v>
       </c>
       <c r="L18">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M18">
         <v>7</v>
@@ -8177,7 +8177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>500</v>
       </c>
       <c r="L19">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M19">
         <v>7</v>
@@ -8233,7 +8233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>500</v>
       </c>
       <c r="L20">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M20">
         <v>7</v>
@@ -8289,7 +8289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>500</v>
       </c>
       <c r="L21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M21">
         <v>7</v>
@@ -8345,7 +8345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8380,7 +8380,7 @@
         <v>500</v>
       </c>
       <c r="L22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M22">
         <v>7</v>
@@ -8401,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>500</v>
       </c>
       <c r="L23">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M23">
         <v>7</v>
@@ -8457,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>500</v>
       </c>
       <c r="L24">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M24">
         <v>7</v>
@@ -8513,7 +8513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>500</v>
       </c>
       <c r="L25">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M25">
         <v>7</v>
@@ -8569,7 +8569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>500</v>
       </c>
       <c r="L26">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M26">
         <v>7</v>
@@ -8625,7 +8625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" ht="28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8660,7 +8660,7 @@
         <v>500</v>
       </c>
       <c r="L27">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M27">
         <v>7</v>
@@ -8692,29 +8692,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E30"/>
+      <selection pane="bottomLeft" activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="16" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="16" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8873,7 +8873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8926,7 +8926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9032,7 +9032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9191,7 +9191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9350,7 +9350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9615,7 +9615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9650,7 +9650,7 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -9668,7 +9668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9703,7 +9703,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -9721,7 +9721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -9774,7 +9774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9809,7 +9809,7 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -9827,7 +9827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9862,7 +9862,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -9880,7 +9880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -9933,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9968,7 +9968,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M24">
         <v>1</v>
@@ -9986,7 +9986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M25">
         <v>1</v>
@@ -10039,7 +10039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10074,7 +10074,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M26">
         <v>1</v>
@@ -10092,7 +10092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10127,7 +10127,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="M27">
         <v>1</v>
@@ -10145,7 +10145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10198,7 +10198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10233,7 +10233,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M29">
         <v>1</v>
@@ -10251,7 +10251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10286,7 +10286,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -10319,23 +10319,23 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
-    <col min="5" max="5" width="19.875" customWidth="1"/>
-    <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
-    <col min="8" max="8" width="11.75" customWidth="1"/>
-    <col min="9" max="9" width="23.125" customWidth="1"/>
-    <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="12" width="11.875" customWidth="1"/>
-    <col min="13" max="13" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="9" max="9" width="23.08984375" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="12" width="11.90625" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -10388,7 +10388,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10441,7 +10441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10653,7 +10653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10706,7 +10706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10759,7 +10759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10812,7 +10812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10865,7 +10865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10986,23 +10986,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
-    <col min="3" max="3" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="21.75" customWidth="1"/>
-    <col min="5" max="5" width="19.875" customWidth="1"/>
-    <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="12.375" customWidth="1"/>
-    <col min="8" max="8" width="11.75" customWidth="1"/>
-    <col min="9" max="9" width="23.125" customWidth="1"/>
-    <col min="10" max="10" width="15.5" customWidth="1"/>
-    <col min="11" max="12" width="11.875" customWidth="1"/>
-    <col min="13" max="13" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" customWidth="1"/>
+    <col min="8" max="8" width="11.7265625" customWidth="1"/>
+    <col min="9" max="9" width="23.08984375" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="12" width="11.90625" customWidth="1"/>
+    <col min="13" max="13" width="11.08984375" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -11055,7 +11055,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11108,7 +11108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11214,7 +11214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11267,7 +11267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11320,7 +11320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11479,7 +11479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11532,7 +11532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" ht="42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11650,26 +11650,26 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.25" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
-    <col min="4" max="4" width="20.125" customWidth="1"/>
-    <col min="5" max="5" width="16.375" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="9" max="9" width="58.125" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="14" width="16.5" customWidth="1"/>
-    <col min="15" max="15" width="12.875" customWidth="1"/>
-    <col min="16" max="17" width="12.625" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.36328125" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" customWidth="1"/>
+    <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="9" max="9" width="58.08984375" customWidth="1"/>
+    <col min="10" max="10" width="38.36328125" customWidth="1"/>
+    <col min="11" max="12" width="12.90625" customWidth="1"/>
+    <col min="13" max="14" width="16.453125" customWidth="1"/>
+    <col min="15" max="15" width="12.90625" customWidth="1"/>
+    <col min="16" max="17" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -11722,7 +11722,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11775,7 +11775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11828,7 +11828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11881,7 +11881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11934,7 +11934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11987,7 +11987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -12040,7 +12040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -12093,7 +12093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -12146,7 +12146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>99</v>
       </c>
       <c r="L10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10">
         <v>1</v>
@@ -12199,7 +12199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -12234,7 +12234,7 @@
         <v>99</v>
       </c>
       <c r="L11">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -12252,7 +12252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -12287,7 +12287,7 @@
         <v>99</v>
       </c>
       <c r="L12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -12305,7 +12305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -12358,7 +12358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -12411,7 +12411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -12464,7 +12464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -12517,7 +12517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="27" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:17" ht="28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -12570,7 +12570,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -12623,7 +12623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -12676,7 +12676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -12729,7 +12729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12782,7 +12782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>

</xml_diff>